<commit_message>
create relational tables, work on process from flat file
</commit_message>
<xml_diff>
--- a/data/fakes.xlsx
+++ b/data/fakes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5EC1F51-895D-0344-9D3B-B20E2A958F6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4326A5-6D2F-224F-AE61-FF16E7657D18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="24600" windowHeight="15460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="24600" windowHeight="15460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="209">
   <si>
     <t>DCBS#</t>
   </si>
@@ -530,9 +530,6 @@
     <t>94 College St</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>name_first</t>
   </si>
   <si>
@@ -593,9 +590,6 @@
     <t>raj</t>
   </si>
   <si>
-    <t>koothrpali</t>
-  </si>
-  <si>
     <t>referral</t>
   </si>
   <si>
@@ -621,12 +615,48 @@
   </si>
   <si>
     <t>perp</t>
+  </si>
+  <si>
+    <t>koothrapali</t>
+  </si>
+  <si>
+    <t>maria</t>
+  </si>
+  <si>
+    <t>gonzalez</t>
+  </si>
+  <si>
+    <t>jesus</t>
+  </si>
+  <si>
+    <t>12 Knight Hall, 400 East College Street, Georgetown, KY</t>
+  </si>
+  <si>
+    <t>25 Knight Hall, 400 East College Street, Georgetown, KY</t>
+  </si>
+  <si>
+    <t>32 Knight Hall, 400 East College Street, Georgetown, KY</t>
+  </si>
+  <si>
+    <t>54 Knight Hall, 400 East College Street, Georgetown, KY</t>
+  </si>
+  <si>
+    <t>200 Dusty Avenue, Mars</t>
+  </si>
+  <si>
+    <t>155 Jackson St, Geogetown</t>
+  </si>
+  <si>
+    <t>230 Malin Avenue, Georgetown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -656,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -665,11 +695,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -680,6 +715,45 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEA4A16F-DB07-974A-A775-531442F9E667}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
+  <autoFilter ref="A1:F11" xr:uid="{D8376242-95EE-E448-96ED-747624C570C6}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E51F2326-687F-8F4C-A7A6-582EB6EB158F}" name="person_id"/>
+    <tableColumn id="2" xr3:uid="{4DDFB2DD-30E3-8746-84E8-8058FAA2A404}" name="name_first"/>
+    <tableColumn id="3" xr3:uid="{82F4E52A-4516-2A4F-9067-419E535DB166}" name="name_last"/>
+    <tableColumn id="4" xr3:uid="{16FC87FF-5280-2848-9773-7BA510C6D17C}" name="DCBS"/>
+    <tableColumn id="5" xr3:uid="{FCD617CF-4C01-BB45-8ADC-0EA5E6060139}" name="address"/>
+    <tableColumn id="6" xr3:uid="{33B87D29-7B16-0643-8075-E34877260B00}" name="dob"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5124C27F-86A5-DC44-941C-DA1A5E514A50}" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{BF8ECD33-A462-C543-A5A2-2AD5DA4D6523}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{EC89D26F-7A41-4648-8B6D-899D00DB3268}" name="referral"/>
+    <tableColumn id="2" xr3:uid="{1A42400E-14E5-5B47-AD10-89294671CDAD}" name="location"/>
+    <tableColumn id="3" xr3:uid="{2F37A77D-7AF5-7C4D-A0AA-23BBEE304C13}" name="date" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2CC7C3EB-5341-4345-84C2-F342D3812DCA}" name="Table3" displayName="Table3" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11" xr:uid="{A0EFFFE7-E580-2F4D-9A67-CA7CC7AC0A1D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{23A5EFA1-DB83-E847-AC21-21EF1D1BD042}" name="person_id"/>
+    <tableColumn id="2" xr3:uid="{58355D2C-A197-B949-B3CE-7D05A23CFD54}" name="referral"/>
+    <tableColumn id="3" xr3:uid="{4C066D37-B219-6B4B-90AB-61D83E8AD42F}" name="role"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3231,32 +3305,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5974153-8AD8-1245-AF4C-9EE806E9A8FC}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" t="s">
         <v>169</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>170</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>171</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>172</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>173</v>
-      </c>
-      <c r="F1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3264,13 +3343,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
         <v>175</v>
-      </c>
-      <c r="C2" t="s">
-        <v>176</v>
       </c>
       <c r="D2">
         <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" s="4">
+        <v>23084</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3278,13 +3363,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" t="s">
         <v>177</v>
-      </c>
-      <c r="C3" t="s">
-        <v>178</v>
       </c>
       <c r="D3">
         <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" s="3">
+        <v>24609</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3292,13 +3383,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" t="s">
         <v>179</v>
-      </c>
-      <c r="C4" t="s">
-        <v>180</v>
       </c>
       <c r="D4">
         <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3306,13 +3400,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" t="s">
         <v>181</v>
-      </c>
-      <c r="C5" t="s">
-        <v>182</v>
       </c>
       <c r="D5">
         <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3320,13 +3417,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
         <v>183</v>
-      </c>
-      <c r="C6" t="s">
-        <v>184</v>
       </c>
       <c r="D6">
         <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3334,13 +3434,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
         <v>185</v>
-      </c>
-      <c r="C7" t="s">
-        <v>186</v>
       </c>
       <c r="D7">
         <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3348,13 +3451,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" t="s">
         <v>187</v>
-      </c>
-      <c r="C8" t="s">
-        <v>188</v>
       </c>
       <c r="D8">
         <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3362,42 +3468,82 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
+      <c r="E9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F67602F-B7B2-8941-B358-FB7229D08305}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
         <v>191</v>
-      </c>
-      <c r="B1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3405,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C2" s="3">
         <v>44243</v>
@@ -3416,36 +3562,75 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C3" s="3">
         <v>43861</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44247</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBB7DD3-F9CC-7948-9B21-8DCE005E8228}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3456,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3467,7 +3652,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3478,7 +3663,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3489,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3500,7 +3685,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3511,7 +3696,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3522,7 +3707,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3533,10 +3718,35 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>198</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>